<commit_message>
0.1.14: Adapt multi-line descriptions.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTsTelegramProcessStructure.xlsx
+++ b/meta/program/BlancoRestGeneratorTsTelegramProcessStructure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163590C9-CB5F-2549-8519-76575A50D616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4506F9-899A-DB4B-AA55-5ED627818B92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="1560" windowWidth="16160" windowHeight="17680" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18460" yWindow="1660" windowWidth="16160" windowHeight="17680" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -328,6 +328,35 @@
     </rPh>
     <rPh sb="14" eb="15">
       <t xml:space="preserve">カカレル </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>descriptionList</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>クラスの補助説明です。文字参照エンコード済みの値を格納してください。</t>
+    <rPh sb="4" eb="6">
+      <t>ホジョ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ズ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>カクノウ</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -751,7 +780,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -886,6 +915,36 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -913,32 +972,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1331,7 +1366,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1375,7 +1410,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1400,10 +1435,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1558,14 +1593,14 @@
       <c r="D16" s="15"/>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -1575,27 +1610,27 @@
       <c r="E18" s="8"/>
       <c r="F18"/>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="61" t="s">
+    <row r="19" spans="1:7">
+      <c r="A19" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="64"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="61"/>
       <c r="F19"/>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="61"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="64"/>
+    <row r="20" spans="1:7">
+      <c r="A20" s="57"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="61"/>
       <c r="F20"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" s="20"/>
       <c r="B21" s="21"/>
       <c r="C21" s="22"/>
@@ -1603,7 +1638,7 @@
       <c r="E21" s="23"/>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22" s="24"/>
       <c r="B22" s="25"/>
       <c r="C22" s="26"/>
@@ -1611,14 +1646,14 @@
       <c r="E22" s="27"/>
       <c r="F22"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="A24" s="4" t="s">
         <v>19</v>
       </c>
@@ -1628,33 +1663,33 @@
       <c r="E24" s="16"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A25" s="61" t="s">
+    <row r="25" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A25" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="65" t="s">
+      <c r="C25" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="65" t="s">
+      <c r="D25" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="65" t="s">
+      <c r="E25" s="58" t="s">
         <v>7</v>
       </c>
       <c r="F25" s="28"/>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="61"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
+    <row r="26" spans="1:7">
+      <c r="A26" s="57"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
       <c r="F26" s="29"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27" s="20">
         <v>1</v>
       </c>
@@ -1670,7 +1705,7 @@
       </c>
       <c r="F27" s="31"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28" s="32">
         <f>A27+1</f>
         <v>2</v>
@@ -1687,195 +1722,195 @@
       </c>
       <c r="F28" s="35"/>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="32">
-        <f t="shared" ref="A29:A41" si="0">A28+1</f>
+    <row r="29" spans="1:7" s="50" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A29" s="71">
+        <f t="shared" ref="A29:A42" si="0">A28+1</f>
         <v>3</v>
       </c>
-      <c r="B29" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="34"/>
-      <c r="E29" s="66" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="67"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="32">
+      <c r="B29" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="63"/>
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="71">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B30" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="45"/>
-      <c r="E30" s="57" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="58"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="32">
+      <c r="B30" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="34"/>
+      <c r="E30" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="54"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="71">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B31" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" s="35"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="32">
+      <c r="B31" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="45"/>
+      <c r="E31" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="68"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="71">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C32" s="34" t="s">
         <v>23</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F32" s="35"/>
     </row>
-    <row r="33" spans="1:7" ht="50" customHeight="1">
-      <c r="A33" s="32">
+    <row r="33" spans="1:7">
+      <c r="A33" s="71">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D33" s="34"/>
-      <c r="E33" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="F33" s="69"/>
-    </row>
-    <row r="34" spans="1:7" s="50" customFormat="1" ht="45">
-      <c r="A34" s="32">
+      <c r="E33" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="35"/>
+    </row>
+    <row r="34" spans="1:7" ht="50" customHeight="1">
+      <c r="A34" s="71">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B34" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="E34" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="F34" s="60"/>
-      <c r="G34"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="32">
+      <c r="B34" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="34"/>
+      <c r="E34" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="56"/>
+    </row>
+    <row r="35" spans="1:7" s="50" customFormat="1" ht="45">
+      <c r="A35" s="71">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B35" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="F35" s="58"/>
-    </row>
-    <row r="36" spans="1:7" s="50" customFormat="1" ht="15">
-      <c r="A36" s="32">
+      <c r="B35" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="70"/>
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="71">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B36" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="C36" s="49" t="s">
+      <c r="B36" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="F36" s="53"/>
-      <c r="G36"/>
+      <c r="D36" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" s="68"/>
     </row>
     <row r="37" spans="1:7" s="50" customFormat="1" ht="15">
-      <c r="A37" s="32">
+      <c r="A37" s="71">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B37" s="48" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C37" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" s="49"/>
-      <c r="E37" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="F37" s="53"/>
+        <v>40</v>
+      </c>
+      <c r="D37" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="63"/>
       <c r="G37"/>
     </row>
-    <row r="38" spans="1:7" s="50" customFormat="1" ht="45" customHeight="1">
-      <c r="A38" s="32">
+    <row r="38" spans="1:7" s="50" customFormat="1" ht="15">
+      <c r="A38" s="71">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B38" s="48" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C38" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="D38" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="E38" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="F38" s="56"/>
+        <v>23</v>
+      </c>
+      <c r="D38" s="49"/>
+      <c r="E38" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="F38" s="63"/>
       <c r="G38"/>
     </row>
-    <row r="39" spans="1:7" s="50" customFormat="1" ht="45">
-      <c r="A39" s="32">
+    <row r="39" spans="1:7" s="50" customFormat="1" ht="45" customHeight="1">
+      <c r="A39" s="71">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B39" s="48" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C39" s="49" t="s">
         <v>52</v>
@@ -1883,19 +1918,19 @@
       <c r="D39" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="52" t="s">
-        <v>64</v>
-      </c>
-      <c r="F39" s="53"/>
+      <c r="E39" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="66"/>
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7" s="50" customFormat="1" ht="45">
-      <c r="A40" s="32">
+      <c r="A40" s="71">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B40" s="48" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C40" s="49" t="s">
         <v>52</v>
@@ -1903,86 +1938,107 @@
       <c r="D40" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="54" t="s">
-        <v>66</v>
-      </c>
-      <c r="F40" s="55"/>
+      <c r="E40" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" s="63"/>
       <c r="G40"/>
     </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="32">
+    <row r="41" spans="1:7" s="50" customFormat="1" ht="45">
+      <c r="A41" s="71">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B41" s="33" t="s">
+      <c r="B41" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="F41" s="65"/>
+      <c r="G41"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="71">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B42" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C42" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="D42" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="E41" s="34" t="s">
+      <c r="E42" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="35"/>
-    </row>
-    <row r="42" spans="1:7" ht="45" customHeight="1">
-      <c r="A42" s="47"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="58"/>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="F42" s="35"/>
+    </row>
+    <row r="43" spans="1:7" ht="45" customHeight="1">
       <c r="A43" s="47"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="46"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="68"/>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="47"/>
-      <c r="B44" s="33"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="35"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="46"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="24"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="37"/>
+      <c r="A45" s="47"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="35"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="24"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E33:F33"/>
+  <mergeCells count="22">
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E34:F34"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="E25:E26"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E29:F29"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">

</xml_diff>